<commit_message>
Update kode. 1. Fungsi keanggotaan nya, Linear Segitiga dan defuzzynya dari weighted average
</commit_message>
<xml_diff>
--- a/hasil_top5.xlsx
+++ b/hasil_top5.xlsx
@@ -467,68 +467,68 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>94</v>
+        <v>16</v>
       </c>
       <c r="B2" t="n">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C2" t="n">
-        <v>52973</v>
+        <v>47217</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>sangat_layak</t>
+          <t>layak</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.8513500000000001</v>
+        <v>0.52</v>
       </c>
       <c r="F2" t="n">
-        <v>85.13500000000001</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>90</v>
+        <v>19</v>
       </c>
       <c r="B3" t="n">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C3" t="n">
-        <v>50325</v>
+        <v>46450</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>sangat_layak</t>
+          <t>layak</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.825</v>
+        <v>0.76</v>
       </c>
       <c r="F3" t="n">
-        <v>82.5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B4" t="n">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C4" t="n">
-        <v>22360</v>
+        <v>47995</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>sangat_layak</t>
+          <t>layak</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.8</v>
+        <v>0.8663333333333333</v>
       </c>
       <c r="F4" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5">
@@ -543,36 +543,36 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>sangat_layak</t>
+          <t>layak</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.7937</v>
+        <v>0.7249333333333333</v>
       </c>
       <c r="F5" t="n">
-        <v>79.36999999999999</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="B6" t="n">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C6" t="n">
-        <v>34513</v>
+        <v>35304</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>sangat_layak</t>
+          <t>layak</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.77435</v>
+        <v>0.9696</v>
       </c>
       <c r="F6" t="n">
-        <v>77.435</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>